<commit_message>
Done the following things:
* read xlxs
  re-wrote, orignial output was a data-frame that wasn't (easy) to index. Wrote a fruntion that put all artists and sons in a list.

* format string
  Created a format string method. Artist and title on top each other and are allwats alligned centerd.

* Made some adjustments to the Xlxs file: added headers.

* from template to pdf
  1- adjust picture to have it stright while printing text and rotate it 90 degrees afterwards.
  2- copied the image part to 'print_bingo_card_image' to experiment how we can best print all values on a bingo card.

* main
  added all the functionalities (that are done) in main
</commit_message>
<xml_diff>
--- a/scraps/titel_artiest_example.xlsx
+++ b/scraps/titel_artiest_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JG\iQuizzen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc3720a8269da2ce/1. Documenten/6. Software projecten/prive/music_bingo/music_bingo/scraps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59224300-FFF1-4CB2-8AE0-5DA181534E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{59224300-FFF1-4CB2-8AE0-5DA181534E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C35E4505-C339-4DCE-8007-3BFBC40B8F33}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{522E6542-9BDE-4F42-9892-028D2BE347B0}"/>
+    <workbookView xWindow="28680" yWindow="4275" windowWidth="29040" windowHeight="15720" xr2:uid="{522E6542-9BDE-4F42-9892-028D2BE347B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,185 +36,199 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t xml:space="preserve">Nirvana </t>
   </si>
   <si>
-    <t xml:space="preserve"> Smells Like Teen Spirit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Britney Spears </t>
   </si>
   <si>
-    <t xml:space="preserve"> ...Baby One More Time</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eminem </t>
   </si>
   <si>
-    <t xml:space="preserve"> Lose Yourself</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spice Girls </t>
   </si>
   <si>
-    <t xml:space="preserve"> Wannabe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Backstreet Boys </t>
   </si>
   <si>
-    <t xml:space="preserve"> I Want It That Way</t>
-  </si>
-  <si>
     <t xml:space="preserve">U2 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Beautiful Day</t>
-  </si>
-  <si>
     <t xml:space="preserve">TLC </t>
   </si>
   <si>
-    <t xml:space="preserve"> Waterfalls</t>
-  </si>
-  <si>
     <t xml:space="preserve">Madonna </t>
   </si>
   <si>
-    <t xml:space="preserve"> Vogue</t>
-  </si>
-  <si>
     <t xml:space="preserve">Radiohead </t>
   </si>
   <si>
-    <t xml:space="preserve"> Creep</t>
-  </si>
-  <si>
     <t xml:space="preserve">Destiny's Child </t>
   </si>
   <si>
-    <t xml:space="preserve"> Say My Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">R.E.M. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Losing My Religion</t>
-  </si>
-  <si>
     <t xml:space="preserve">OutKast </t>
   </si>
   <si>
-    <t xml:space="preserve"> Hey Ya!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Whitney Houston </t>
   </si>
   <si>
-    <t xml:space="preserve"> I Will Always Love You</t>
-  </si>
-  <si>
     <t xml:space="preserve">Oasis </t>
   </si>
   <si>
-    <t xml:space="preserve"> Wonderwall</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mariah Carey </t>
   </si>
   <si>
-    <t xml:space="preserve"> Vision of Love</t>
-  </si>
-  <si>
     <t xml:space="preserve">Green Day </t>
   </si>
   <si>
-    <t xml:space="preserve"> Basket Case</t>
-  </si>
-  <si>
     <t xml:space="preserve">No Doubt </t>
   </si>
   <si>
-    <t xml:space="preserve"> Don't Speak</t>
-  </si>
-  <si>
     <t xml:space="preserve">2Pac </t>
   </si>
   <si>
-    <t xml:space="preserve"> California Love</t>
-  </si>
-  <si>
     <t xml:space="preserve">NSYNC </t>
   </si>
   <si>
-    <t xml:space="preserve"> Bye Bye Bye</t>
-  </si>
-  <si>
     <t xml:space="preserve">Red Hot Chili Peppers </t>
   </si>
   <si>
-    <t xml:space="preserve"> Under the Bridge</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jennifer Lopez </t>
   </si>
   <si>
-    <t xml:space="preserve"> Jenny From the Block</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alanis Morissette </t>
   </si>
   <si>
-    <t xml:space="preserve"> You Oughta Know</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Notorious B.I.G. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Mo Money Mo Problems</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coldplay </t>
   </si>
   <si>
-    <t xml:space="preserve"> Yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> No Scrubs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Christina Aguilera </t>
   </si>
   <si>
-    <t xml:space="preserve"> Genie in a Bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> All the Small Things</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Like a Prayer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Always Be My Baby</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nelly </t>
   </si>
   <si>
     <t>Blink-182</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hot in Here</t>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Artiest</t>
+  </si>
+  <si>
+    <t>Wannabe</t>
+  </si>
+  <si>
+    <t>Waterfalls</t>
+  </si>
+  <si>
+    <t>Vogue</t>
+  </si>
+  <si>
+    <t>Creep</t>
+  </si>
+  <si>
+    <t>Wonderwall</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Smells Like Teen Spirit</t>
+  </si>
+  <si>
+    <t>...Baby One More Time</t>
+  </si>
+  <si>
+    <t>Lose Yourself</t>
+  </si>
+  <si>
+    <t>I Want It That Way</t>
+  </si>
+  <si>
+    <t>Beautiful Day</t>
+  </si>
+  <si>
+    <t>Say My Name</t>
+  </si>
+  <si>
+    <t>Losing My Religion</t>
+  </si>
+  <si>
+    <t>Hey Ya!</t>
+  </si>
+  <si>
+    <t>I Will Always Love You</t>
+  </si>
+  <si>
+    <t>Vision of Love</t>
+  </si>
+  <si>
+    <t>Basket Case</t>
+  </si>
+  <si>
+    <t>Don't Speak</t>
+  </si>
+  <si>
+    <t>California Love</t>
+  </si>
+  <si>
+    <t>Bye Bye Bye</t>
+  </si>
+  <si>
+    <t>Under the Bridge</t>
+  </si>
+  <si>
+    <t>Jenny From the Block</t>
+  </si>
+  <si>
+    <t>You Oughta Know</t>
+  </si>
+  <si>
+    <t>Mo Money Mo Problems</t>
+  </si>
+  <si>
+    <t>No Scrubs</t>
+  </si>
+  <si>
+    <t>Genie in a Bottle</t>
+  </si>
+  <si>
+    <t>All the Small Things</t>
+  </si>
+  <si>
+    <t>Like a Prayer</t>
+  </si>
+  <si>
+    <t>Always Be My Baby</t>
+  </si>
+  <si>
+    <t>Hot in Here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -242,8 +256,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,259 +573,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2A4C2D-CB38-4DFF-9A79-821631B291D8}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
applied Juliens feedback and worked on printing values on the image or pdf.
</commit_message>
<xml_diff>
--- a/scraps/titel_artiest_example.xlsx
+++ b/scraps/titel_artiest_example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{59224300-FFF1-4CB2-8AE0-5DA181534E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C35E4505-C339-4DCE-8007-3BFBC40B8F33}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4275" windowWidth="29040" windowHeight="15720" xr2:uid="{522E6542-9BDE-4F42-9892-028D2BE347B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{522E6542-9BDE-4F42-9892-028D2BE347B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>